<commit_message>
fix typos in source data
</commit_message>
<xml_diff>
--- a/source_data/50_data.xlsx
+++ b/source_data/50_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingyan.hu\Downloads\Step2_MinSetStaticCopy_reformat&amp;upload\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\source_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E32EA49-8706-40BB-B6BD-F7AFEF60D752}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B946BAC-1883-4C14-A602-18CC0C6DF5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-54120" yWindow="-1320" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_50_data " sheetId="1" r:id="rId1"/>
@@ -1292,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB67"/>
+  <dimension ref="A1:AA67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1321,6 @@
     <col min="25" max="25" width="39.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="39.5703125" style="3" customWidth="1"/>
     <col min="27" max="27" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">

</xml_diff>